<commit_message>
implementar reporte excel en kardex
</commit_message>
<xml_diff>
--- a/public/reporte-por-area.xlsx
+++ b/public/reporte-por-area.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="38">
   <si>
     <t>ID</t>
   </si>
@@ -50,7 +50,7 @@
     <t>TEXTO</t>
   </si>
   <si>
-    <t>GRAPAS DE METAL 26/6 CAJA X 5000</t>
+    <t>ARCHIVADOR DE CARTON PLASTIFICADO CON PALANCA LOMO ANCHO TAMAÑO A4 - ARTESCO</t>
   </si>
   <si>
     <t>UND</t>
@@ -59,70 +59,76 @@
     <t>UTILES DE ESCRITORIO</t>
   </si>
   <si>
-    <t>ARCHIVO</t>
-  </si>
-  <si>
-    <t>CARGO-0488</t>
-  </si>
-  <si>
-    <t>RECIBIO ALBERTO</t>
-  </si>
-  <si>
-    <t>RESALTADOR VERDE</t>
+    <t>FARMACIA</t>
+  </si>
+  <si>
+    <t>8MI02J</t>
+  </si>
+  <si>
+    <t>PARA FARMACIA / DR ALEX/CARGO-0987</t>
+  </si>
+  <si>
+    <t>MICA OFICIO PQT X 10</t>
+  </si>
+  <si>
+    <t>G37QCJ</t>
+  </si>
+  <si>
+    <t>PARA FARMACIA /MARTHA/CARGO-0930</t>
+  </si>
+  <si>
+    <t>PAPEL BOND 75g TAMAÑO A4 - KERO (PQT x 500)</t>
+  </si>
+  <si>
+    <t>LDIZTL</t>
+  </si>
+  <si>
+    <t>PARA FARMACIA /DR ALEX/CARGO-0831</t>
+  </si>
+  <si>
+    <t>PLUMON TINTA INDELEBLE MARCADOR AZUL PUNTA FINA</t>
+  </si>
+  <si>
+    <t>AEVOMH</t>
+  </si>
+  <si>
+    <t>PARA FARMACIA /DR ALEX/CARGO-0804</t>
+  </si>
+  <si>
+    <t>BANDERITA SEÑALIZADORA 4.30 cm x 2.54 cm APROX x 50 HOJAS COLOR AMARILLO</t>
+  </si>
+  <si>
+    <t>30FC3F</t>
+  </si>
+  <si>
+    <t>PARA FARMACIA /MARTHA/CARGO-0788</t>
   </si>
   <si>
     <t>BOLIGRAFO (LAPICERO) DE TINTA SECA PUNTA FINA COLOR AZUL</t>
   </si>
   <si>
-    <t>BORRADOR BLANCO PARA LAPIZ TAMAÑO GRANDE</t>
-  </si>
-  <si>
-    <t>NOTAS ADHESIVAS 3 X 2 (50 X 75 MM) - 100 HOJAS ARTESCO</t>
-  </si>
-  <si>
-    <t>CARGO-0489</t>
-  </si>
-  <si>
-    <t>CORRECTOR LIQUIDO TIPO LAPICERO CON PUNTA FINA DE METAL</t>
-  </si>
-  <si>
-    <t>RESALTADOR AMARILLO</t>
+    <t>BOLIGRAFO (LAPICERO) DE TINTA SECA PUNTA FINA COLOR NEGRO</t>
   </si>
   <si>
     <t>CUADERNO CUADRICULADO TAMAÑO A4 X 92 HOJAS</t>
   </si>
   <si>
-    <t>BOLIGRAFO (LAPICERO) DE TINTA SECA PUNTA FINA COLOR ROJO</t>
-  </si>
-  <si>
-    <t>FOLDER MANILA OFICIO</t>
-  </si>
-  <si>
-    <t>PAPEL BULKY 52g TAMAÑO A4 - GRAPHOS (PQT x 500)</t>
-  </si>
-  <si>
-    <t>PQT</t>
-  </si>
-  <si>
-    <t>CLIP DE METAL 33 MM CAJA X 100 UND</t>
-  </si>
-  <si>
-    <t>LAPIZ 2B</t>
-  </si>
-  <si>
-    <t>USB 64 GB</t>
-  </si>
-  <si>
-    <t>BOLIGRAFO (LAPICERO) DE TINTA SECA PUNTA FINA COLOR NEGRO</t>
-  </si>
-  <si>
-    <t>FASTER DE METAL CAJA X 50 UND</t>
-  </si>
-  <si>
-    <t>TAJADOR DE METAL</t>
-  </si>
-  <si>
-    <t>PAPEL BOND 75g TAMAÑO A4 - KERO (PQT x 500)</t>
+    <t>SUHYV3</t>
+  </si>
+  <si>
+    <t>PARA FARMACIA / DR ALEX/CARGO-0784</t>
+  </si>
+  <si>
+    <t>S7245X</t>
+  </si>
+  <si>
+    <t>PARA FARMACIA / DR ALEX/CARGO-0778</t>
+  </si>
+  <si>
+    <t>J0TOH2</t>
+  </si>
+  <si>
+    <t>PARA FARMACIA-SANDRA /PATY/CARGO-0760</t>
   </si>
 </sst>
 </file>
@@ -465,25 +471,25 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:K19"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="4.57" bestFit="true" customWidth="true" style="0"/>
     <col min="2" max="2" width="15.282" bestFit="true" customWidth="true" style="0"/>
-    <col min="3" max="3" width="68.269" bestFit="true" customWidth="true" style="0"/>
+    <col min="3" max="3" width="90.692" bestFit="true" customWidth="true" style="0"/>
     <col min="4" max="4" width="4.57" bestFit="true" customWidth="true" style="0"/>
     <col min="5" max="5" width="5.856" bestFit="true" customWidth="true" style="0"/>
     <col min="6" max="6" width="5.856" bestFit="true" customWidth="true" style="0"/>
     <col min="7" max="7" width="24.708" bestFit="true" customWidth="true" style="0"/>
-    <col min="8" max="8" width="9.283" bestFit="true" customWidth="true" style="0"/>
+    <col min="8" max="8" width="10.569" bestFit="true" customWidth="true" style="0"/>
     <col min="9" max="9" width="12.854" bestFit="true" customWidth="true" style="0"/>
     <col min="10" max="10" width="15.282" bestFit="true" customWidth="true" style="0"/>
-    <col min="11" max="11" width="18.71" bestFit="true" customWidth="true" style="0"/>
+    <col min="11" max="11" width="44.703" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -523,10 +529,10 @@
     </row>
     <row r="2" spans="1:11">
       <c r="A2">
-        <v>161</v>
+        <v>342</v>
       </c>
       <c r="B2">
-        <v>718500080026</v>
+        <v>710600010098</v>
       </c>
       <c r="C2" t="s">
         <v>11</v>
@@ -535,7 +541,7 @@
         <v>12</v>
       </c>
       <c r="E2">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="F2"/>
       <c r="G2" t="s">
@@ -548,7 +554,7 @@
         <v>15</v>
       </c>
       <c r="J2" s="1">
-        <v>45139.0</v>
+        <v>45621.0</v>
       </c>
       <c r="K2" t="s">
         <v>16</v>
@@ -556,10 +562,10 @@
     </row>
     <row r="3" spans="1:11">
       <c r="A3">
-        <v>202</v>
+        <v>174</v>
       </c>
       <c r="B3">
-        <v>716000060445</v>
+        <v>710600120058</v>
       </c>
       <c r="C3" t="s">
         <v>17</v>
@@ -568,7 +574,7 @@
         <v>12</v>
       </c>
       <c r="E3">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="F3"/>
       <c r="G3" t="s">
@@ -578,30 +584,30 @@
         <v>14</v>
       </c>
       <c r="I3" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="J3" s="1">
-        <v>45139.0</v>
+        <v>45579.0</v>
       </c>
       <c r="K3" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4">
-        <v>275</v>
+        <v>6</v>
       </c>
       <c r="B4">
-        <v>716000010208</v>
+        <v>717200050136</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D4" t="s">
         <v>12</v>
       </c>
       <c r="E4">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F4"/>
       <c r="G4" t="s">
@@ -611,24 +617,24 @@
         <v>14</v>
       </c>
       <c r="I4" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="J4" s="1">
-        <v>45139.0</v>
+        <v>45505.0</v>
       </c>
       <c r="K4" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:11">
       <c r="A5">
-        <v>278</v>
+        <v>170</v>
       </c>
       <c r="B5">
-        <v>711100010036</v>
+        <v>716000060410</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
@@ -644,30 +650,30 @@
         <v>14</v>
       </c>
       <c r="I5" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="J5" s="1">
-        <v>45139.0</v>
+        <v>45475.0</v>
       </c>
       <c r="K5" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:11">
       <c r="A6">
-        <v>177</v>
+        <v>226</v>
       </c>
       <c r="B6">
-        <v>710300120048</v>
+        <v>710300130036</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="D6" t="s">
         <v>12</v>
       </c>
       <c r="E6">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F6"/>
       <c r="G6" t="s">
@@ -677,30 +683,30 @@
         <v>14</v>
       </c>
       <c r="I6" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="J6" s="1">
-        <v>45139.0</v>
+        <v>45468.0</v>
       </c>
       <c r="K6" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:11">
       <c r="A7">
-        <v>143</v>
+        <v>275</v>
       </c>
       <c r="B7">
-        <v>711100030001</v>
+        <v>716000010208</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D7" t="s">
         <v>12</v>
       </c>
       <c r="E7">
-        <v>12</v>
+        <v>50</v>
       </c>
       <c r="F7"/>
       <c r="G7" t="s">
@@ -710,30 +716,30 @@
         <v>14</v>
       </c>
       <c r="I7" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="J7" s="1">
-        <v>45139.0</v>
+        <v>45468.0</v>
       </c>
       <c r="K7" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:11">
       <c r="A8">
-        <v>199</v>
+        <v>276</v>
       </c>
       <c r="B8">
-        <v>716000060443</v>
+        <v>716000010209</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D8" t="s">
         <v>12</v>
       </c>
       <c r="E8">
-        <v>12</v>
+        <v>50</v>
       </c>
       <c r="F8"/>
       <c r="G8" t="s">
@@ -743,13 +749,13 @@
         <v>14</v>
       </c>
       <c r="I8" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="J8" s="1">
-        <v>45139.0</v>
+        <v>45468.0</v>
       </c>
       <c r="K8" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -760,7 +766,7 @@
         <v>717200030125</v>
       </c>
       <c r="C9" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="D9" t="s">
         <v>12</v>
@@ -776,30 +782,30 @@
         <v>14</v>
       </c>
       <c r="I9" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="J9" s="1">
-        <v>45139.0</v>
+        <v>45463.0</v>
       </c>
       <c r="K9" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:11">
       <c r="A10">
-        <v>277</v>
+        <v>6</v>
       </c>
       <c r="B10">
-        <v>716000010187</v>
+        <v>717200050136</v>
       </c>
       <c r="C10" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D10" t="s">
         <v>12</v>
       </c>
       <c r="E10">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="F10"/>
       <c r="G10" t="s">
@@ -809,30 +815,30 @@
         <v>14</v>
       </c>
       <c r="I10" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="J10" s="1">
-        <v>45139.0</v>
+        <v>45460.0</v>
       </c>
       <c r="K10" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:11">
       <c r="A11">
-        <v>155</v>
+        <v>258</v>
       </c>
       <c r="B11">
-        <v>710600040025</v>
+        <v>717200030125</v>
       </c>
       <c r="C11" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="D11" t="s">
         <v>12</v>
       </c>
       <c r="E11">
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="F11"/>
       <c r="G11" t="s">
@@ -842,277 +848,13 @@
         <v>14</v>
       </c>
       <c r="I11" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="J11" s="1">
-        <v>45139.0</v>
+        <v>45449.0</v>
       </c>
       <c r="K11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11">
-      <c r="A12">
-        <v>2</v>
-      </c>
-      <c r="B12">
-        <v>717200330039</v>
-      </c>
-      <c r="C12" t="s">
-        <v>27</v>
-      </c>
-      <c r="D12" t="s">
-        <v>28</v>
-      </c>
-      <c r="E12">
-        <v>6</v>
-      </c>
-      <c r="F12"/>
-      <c r="G12" t="s">
-        <v>13</v>
-      </c>
-      <c r="H12" t="s">
-        <v>14</v>
-      </c>
-      <c r="I12" t="s">
-        <v>15</v>
-      </c>
-      <c r="J12" s="1">
-        <v>45139.0</v>
-      </c>
-      <c r="K12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11">
-      <c r="A13">
-        <v>136</v>
-      </c>
-      <c r="B13">
-        <v>718500050001</v>
-      </c>
-      <c r="C13" t="s">
-        <v>29</v>
-      </c>
-      <c r="D13" t="s">
-        <v>12</v>
-      </c>
-      <c r="E13">
-        <v>6</v>
-      </c>
-      <c r="F13"/>
-      <c r="G13" t="s">
-        <v>13</v>
-      </c>
-      <c r="H13" t="s">
-        <v>14</v>
-      </c>
-      <c r="I13" t="s">
-        <v>15</v>
-      </c>
-      <c r="J13" s="1">
-        <v>45139.0</v>
-      </c>
-      <c r="K13" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11">
-      <c r="A14">
-        <v>167</v>
-      </c>
-      <c r="B14">
-        <v>716000040112</v>
-      </c>
-      <c r="C14" t="s">
-        <v>30</v>
-      </c>
-      <c r="D14" t="s">
-        <v>12</v>
-      </c>
-      <c r="E14">
-        <v>6</v>
-      </c>
-      <c r="F14"/>
-      <c r="G14" t="s">
-        <v>13</v>
-      </c>
-      <c r="H14" t="s">
-        <v>14</v>
-      </c>
-      <c r="I14" t="s">
-        <v>15</v>
-      </c>
-      <c r="J14" s="1">
-        <v>45139.0</v>
-      </c>
-      <c r="K14" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11">
-      <c r="A15">
-        <v>223</v>
-      </c>
-      <c r="B15">
-        <v>767500590014</v>
-      </c>
-      <c r="C15" t="s">
-        <v>31</v>
-      </c>
-      <c r="D15" t="s">
-        <v>12</v>
-      </c>
-      <c r="E15">
-        <v>1</v>
-      </c>
-      <c r="F15"/>
-      <c r="G15" t="s">
-        <v>13</v>
-      </c>
-      <c r="H15" t="s">
-        <v>14</v>
-      </c>
-      <c r="I15" t="s">
-        <v>15</v>
-      </c>
-      <c r="J15" s="1">
-        <v>45139.0</v>
-      </c>
-      <c r="K15" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11">
-      <c r="A16">
-        <v>276</v>
-      </c>
-      <c r="B16">
-        <v>716000010209</v>
-      </c>
-      <c r="C16" t="s">
-        <v>32</v>
-      </c>
-      <c r="D16" t="s">
-        <v>12</v>
-      </c>
-      <c r="E16">
-        <v>18</v>
-      </c>
-      <c r="F16"/>
-      <c r="G16" t="s">
-        <v>13</v>
-      </c>
-      <c r="H16" t="s">
-        <v>14</v>
-      </c>
-      <c r="I16" t="s">
-        <v>15</v>
-      </c>
-      <c r="J16" s="1">
-        <v>45139.0</v>
-      </c>
-      <c r="K16" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11">
-      <c r="A17">
-        <v>151</v>
-      </c>
-      <c r="B17">
-        <v>718500100014</v>
-      </c>
-      <c r="C17" t="s">
-        <v>33</v>
-      </c>
-      <c r="D17" t="s">
-        <v>12</v>
-      </c>
-      <c r="E17">
-        <v>50</v>
-      </c>
-      <c r="F17"/>
-      <c r="G17" t="s">
-        <v>13</v>
-      </c>
-      <c r="H17" t="s">
-        <v>14</v>
-      </c>
-      <c r="I17" t="s">
-        <v>21</v>
-      </c>
-      <c r="J17" s="1">
-        <v>45139.0</v>
-      </c>
-      <c r="K17" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11">
-      <c r="A18">
-        <v>209</v>
-      </c>
-      <c r="B18">
-        <v>715000220029</v>
-      </c>
-      <c r="C18" t="s">
-        <v>34</v>
-      </c>
-      <c r="D18" t="s">
-        <v>12</v>
-      </c>
-      <c r="E18">
-        <v>1</v>
-      </c>
-      <c r="F18"/>
-      <c r="G18" t="s">
-        <v>13</v>
-      </c>
-      <c r="H18" t="s">
-        <v>14</v>
-      </c>
-      <c r="I18" t="s">
-        <v>21</v>
-      </c>
-      <c r="J18" s="1">
-        <v>45139.0</v>
-      </c>
-      <c r="K18" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11">
-      <c r="A19">
-        <v>6</v>
-      </c>
-      <c r="B19">
-        <v>717200050136</v>
-      </c>
-      <c r="C19" t="s">
-        <v>35</v>
-      </c>
-      <c r="D19" t="s">
-        <v>12</v>
-      </c>
-      <c r="E19">
-        <v>10</v>
-      </c>
-      <c r="F19"/>
-      <c r="G19" t="s">
-        <v>13</v>
-      </c>
-      <c r="H19" t="s">
-        <v>14</v>
-      </c>
-      <c r="I19" t="s">
-        <v>15</v>
-      </c>
-      <c r="J19" s="1">
-        <v>45139.0</v>
-      </c>
-      <c r="K19" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>